<commit_message>
Added BSP files for audio handling. Basic functions created however, unused and without prototype
</commit_message>
<xml_diff>
--- a/ORDERS.xlsx
+++ b/ORDERS.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pieter Goos\Google Drive\Stellenbosch University\5th Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35003A7E-54AB-43CD-8369-440824DA066C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269A973D-FE25-4D98-AAAA-5C82CEFAC90D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9428" yWindow="-495" windowWidth="21600" windowHeight="11422" xr2:uid="{2174472C-7489-4BDC-8105-73483BCB5CCC}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11423" activeTab="2" xr2:uid="{2174472C-7489-4BDC-8105-73483BCB5CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
   <si>
     <t>Part Number</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Can be any SMT 6x6mm button that is 5mm high</t>
+  </si>
+  <si>
+    <t>Texas Instruments TLV75533PDBVR</t>
+  </si>
+  <si>
+    <t>USB-A-S-F-B-VU</t>
   </si>
 </sst>
 </file>
@@ -705,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE3D6F4-AE96-40CE-929E-7D6CD7BE210C}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1428,4 +1434,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E76779-C18C-46D8-83D0-EC7E18A69C6A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Basic File Reading working and audio scheduling correct. Gibberish output
</commit_message>
<xml_diff>
--- a/ORDERS.xlsx
+++ b/ORDERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pieter Goos\Google Drive\Stellenbosch University\5th Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269A973D-FE25-4D98-AAAA-5C82CEFAC90D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431099FE-A07C-4EF9-9CA5-421A700A1974}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11423" activeTab="2" xr2:uid="{2174472C-7489-4BDC-8105-73483BCB5CCC}"/>
+    <workbookView xWindow="2377" yWindow="10470" windowWidth="21600" windowHeight="11423" activeTab="2" xr2:uid="{2174472C-7489-4BDC-8105-73483BCB5CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
   <si>
     <t>Part Number</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>USB-A-S-F-B-VU</t>
+  </si>
+  <si>
+    <t>CUI SJ1-3533NG</t>
+  </si>
+  <si>
+    <t>ST NUCLEO-F767ZI</t>
+  </si>
+  <si>
+    <t>Davies Molding 1101-A</t>
   </si>
 </sst>
 </file>
@@ -1438,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E76779-C18C-46D8-83D0-EC7E18A69C6A}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1456,6 +1465,21 @@
         <v>98</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>